<commit_message>
update base CSV to save new checkins
</commit_message>
<xml_diff>
--- a/post-checkin/checkin_statistics.xlsx
+++ b/post-checkin/checkin_statistics.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
+    <sheet name="Not Checked In" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Metric</t>
   </si>
@@ -28,6 +29,63 @@
     <t>Count</t>
   </si>
   <si>
+    <t>Total Checked In</t>
+  </si>
+  <si>
+    <t>Males Checked In</t>
+  </si>
+  <si>
+    <t>Females Checked In</t>
+  </si>
+  <si>
+    <t>Adults Checked In</t>
+  </si>
+  <si>
+    <t>Grade Infant/ShishuVihar</t>
+  </si>
+  <si>
+    <t>Grade Pre-KG</t>
+  </si>
+  <si>
+    <t>Grade KG</t>
+  </si>
+  <si>
+    <t>Grade 1</t>
+  </si>
+  <si>
+    <t>Grade 2</t>
+  </si>
+  <si>
+    <t>Grade 3</t>
+  </si>
+  <si>
+    <t>Grade 4</t>
+  </si>
+  <si>
+    <t>Grade 5</t>
+  </si>
+  <si>
+    <t>Grade 6</t>
+  </si>
+  <si>
+    <t>Grade 7</t>
+  </si>
+  <si>
+    <t>Grade 8</t>
+  </si>
+  <si>
+    <t>Grade 9</t>
+  </si>
+  <si>
+    <t>Grade 10</t>
+  </si>
+  <si>
+    <t>Grade 11</t>
+  </si>
+  <si>
+    <t>Grade 12</t>
+  </si>
+  <si>
     <t>Total Not Checked In</t>
   </si>
   <si>
@@ -38,63 +96,6 @@
   </si>
   <si>
     <t>Adults Not Checked In</t>
-  </si>
-  <si>
-    <t>Grade Infant/ShishuVihar</t>
-  </si>
-  <si>
-    <t>Grade Pre-KG</t>
-  </si>
-  <si>
-    <t>Grade KG</t>
-  </si>
-  <si>
-    <t>Grade 1</t>
-  </si>
-  <si>
-    <t>Grade 2</t>
-  </si>
-  <si>
-    <t>Grade 3</t>
-  </si>
-  <si>
-    <t>Grade 4</t>
-  </si>
-  <si>
-    <t>Grade 5</t>
-  </si>
-  <si>
-    <t>Grade 6</t>
-  </si>
-  <si>
-    <t>Grade 7</t>
-  </si>
-  <si>
-    <t>Grade 8</t>
-  </si>
-  <si>
-    <t>Grade 9</t>
-  </si>
-  <si>
-    <t>Grade 10</t>
-  </si>
-  <si>
-    <t>Grade 11</t>
-  </si>
-  <si>
-    <t>Grade 12</t>
-  </si>
-  <si>
-    <t>Check-in Percentage</t>
-  </si>
-  <si>
-    <t>San Jose - Not Checked In</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>60.3%</t>
   </si>
 </sst>
 </file>
@@ -452,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,13 +478,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>161</v>
+        <v>244</v>
       </c>
       <c r="C2">
-        <v>205</v>
+        <v>311</v>
       </c>
       <c r="D2">
-        <v>366</v>
+        <v>555</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -491,13 +492,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>161</v>
+        <v>244</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>161</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -508,10 +509,10 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>205</v>
+        <v>311</v>
       </c>
       <c r="D4">
-        <v>205</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -519,13 +520,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>141</v>
+        <v>203</v>
       </c>
       <c r="C5">
-        <v>168</v>
+        <v>271</v>
       </c>
       <c r="D5">
-        <v>309</v>
+        <v>474</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -533,13 +534,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -547,10 +548,10 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -561,13 +562,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -575,13 +576,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -592,10 +593,10 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -603,13 +604,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -617,13 +618,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -631,13 +632,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -645,13 +646,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -659,13 +660,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -673,13 +674,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -690,10 +691,10 @@
         <v>4</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -701,13 +702,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -715,13 +716,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -729,6 +730,299 @@
         <v>22</v>
       </c>
       <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>161</v>
+      </c>
+      <c r="C2">
+        <v>205</v>
+      </c>
+      <c r="D2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>161</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>205</v>
+      </c>
+      <c r="D4">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>141</v>
+      </c>
+      <c r="C5">
+        <v>168</v>
+      </c>
+      <c r="D5">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
@@ -736,34 +1030,6 @@
       </c>
       <c r="D20">
         <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>